<commit_message>
Fixed Dev Gantt diagram
</commit_message>
<xml_diff>
--- a/pp/gantt/DevGantt.xlsx
+++ b/pp/gantt/DevGantt.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -446,7 +446,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -574,13 +574,13 @@
       </c>
       <c r="E5" t="str">
         <f t="shared" si="0"/>
-        <v>10g</v>
+        <v>25g</v>
       </c>
       <c r="F5" s="2">
-        <v>42765.333333333336</v>
+        <v>42779.333333333336</v>
       </c>
       <c r="G5" s="2">
-        <v>42776.666666666664</v>
+        <v>42811.666666666664</v>
       </c>
       <c r="I5">
         <v>2</v>

</xml_diff>